<commit_message>
hotfix header link for bemeqi
</commit_message>
<xml_diff>
--- a/src/frontend/public/assets/files/ProtocoloMEQI.xlsx
+++ b/src/frontend/public/assets/files/ProtocoloMEQI.xlsx
@@ -248,7 +248,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -341,12 +341,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -528,7 +522,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -633,7 +627,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,11 +639,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -657,12 +651,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -834,7 +824,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>448200</xdr:colOff>
+      <xdr:colOff>447480</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -850,7 +840,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="7268760"/>
-          <a:ext cx="2078280" cy="0"/>
+          <a:ext cx="2077560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -871,7 +861,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>627480</xdr:colOff>
+      <xdr:colOff>626760</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -887,7 +877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="7459200"/>
-          <a:ext cx="7338240" cy="0"/>
+          <a:ext cx="7337520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -908,7 +898,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>683640</xdr:colOff>
+      <xdr:colOff>682920</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -924,7 +914,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9646560" y="7459200"/>
-          <a:ext cx="2999880" cy="0"/>
+          <a:ext cx="2999160" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -945,7 +935,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>190440</xdr:colOff>
+      <xdr:colOff>189720</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -961,7 +951,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10521360" y="7459200"/>
-          <a:ext cx="7517160" cy="0"/>
+          <a:ext cx="7516440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -982,7 +972,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>16920</xdr:colOff>
+      <xdr:colOff>16200</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -998,7 +988,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14173920" y="7459200"/>
-          <a:ext cx="3002040" cy="0"/>
+          <a:ext cx="3001320" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1019,7 +1009,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>726840</xdr:colOff>
+      <xdr:colOff>726120</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1035,7 +1025,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15193440" y="7459200"/>
-          <a:ext cx="7515360" cy="0"/>
+          <a:ext cx="7514640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1056,7 +1046,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>191520</xdr:colOff>
+      <xdr:colOff>190800</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1072,7 +1062,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18483120" y="7459200"/>
-          <a:ext cx="3001320" cy="0"/>
+          <a:ext cx="3000600" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1093,7 +1083,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>1413720</xdr:colOff>
+      <xdr:colOff>1413000</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1109,7 +1099,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="19378080" y="7459200"/>
-          <a:ext cx="7515000" cy="0"/>
+          <a:ext cx="7514280" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1130,7 +1120,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>189720</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1146,7 +1136,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="22667760" y="7459200"/>
-          <a:ext cx="3001320" cy="0"/>
+          <a:ext cx="3000600" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1167,7 +1157,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>722880</xdr:colOff>
+      <xdr:colOff>722160</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1183,7 +1173,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="25682400" y="7459200"/>
-          <a:ext cx="7515000" cy="0"/>
+          <a:ext cx="7514280" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1204,7 +1194,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
+      <xdr:colOff>239760</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1220,7 +1210,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="33211080" y="7459200"/>
-          <a:ext cx="3001680" cy="0"/>
+          <a:ext cx="3000960" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1241,7 +1231,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>774000</xdr:colOff>
+      <xdr:colOff>773280</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1257,7 +1247,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="36226440" y="7459200"/>
-          <a:ext cx="7515000" cy="0"/>
+          <a:ext cx="7514280" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1278,7 +1268,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290520</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1294,7 +1284,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="43754760" y="7459200"/>
-          <a:ext cx="3001320" cy="0"/>
+          <a:ext cx="3000600" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1315,7 +1305,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>1748160</xdr:colOff>
+      <xdr:colOff>1747440</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1331,7 +1321,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="46769760" y="7459200"/>
-          <a:ext cx="8438400" cy="0"/>
+          <a:ext cx="8437680" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1352,7 +1342,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>342000</xdr:colOff>
+      <xdr:colOff>341280</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1368,7 +1358,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="55221480" y="7459200"/>
-          <a:ext cx="2078280" cy="0"/>
+          <a:ext cx="2077560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1389,7 +1379,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
+      <xdr:colOff>49320</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1405,7 +1395,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="57313440" y="7459200"/>
-          <a:ext cx="8438040" cy="0"/>
+          <a:ext cx="8437320" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1426,7 +1416,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
-      <xdr:colOff>392760</xdr:colOff>
+      <xdr:colOff>392040</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1442,7 +1432,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="65764800" y="7459200"/>
-          <a:ext cx="2078280" cy="0"/>
+          <a:ext cx="2077560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1463,7 +1453,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>54</xdr:col>
-      <xdr:colOff>100800</xdr:colOff>
+      <xdr:colOff>100080</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1479,7 +1469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="67856760" y="7459200"/>
-          <a:ext cx="8438400" cy="0"/>
+          <a:ext cx="8437680" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1500,7 +1490,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>448200</xdr:colOff>
+      <xdr:colOff>447480</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1516,7 +1506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="8030880"/>
-          <a:ext cx="2078280" cy="0"/>
+          <a:ext cx="2077560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1537,7 +1527,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>191880</xdr:colOff>
+      <xdr:colOff>191160</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1553,7 +1543,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="8030880"/>
-          <a:ext cx="8260200" cy="0"/>
+          <a:ext cx="8259480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1574,7 +1564,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>448200</xdr:colOff>
+      <xdr:colOff>447480</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1590,7 +1580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="8030880"/>
-          <a:ext cx="2078280" cy="0"/>
+          <a:ext cx="2077560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,7 +1601,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>191880</xdr:colOff>
+      <xdr:colOff>191160</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1627,7 +1617,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="8030880"/>
-          <a:ext cx="8260200" cy="0"/>
+          <a:ext cx="8259480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1648,7 +1638,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>448200</xdr:colOff>
+      <xdr:colOff>447480</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1664,7 +1654,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="8602200"/>
-          <a:ext cx="2078280" cy="0"/>
+          <a:ext cx="2077560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1685,7 +1675,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>191880</xdr:colOff>
+      <xdr:colOff>191160</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1701,7 +1691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3080880" y="8602200"/>
-          <a:ext cx="8260200" cy="0"/>
+          <a:ext cx="8259480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2873,12 +2863,12 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="22.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2995,7 +2985,7 @@
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
         <v>69</v>
       </c>
@@ -3005,7 +2995,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
         <v>58</v>
       </c>
@@ -3028,7 +3018,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="s">
         <v>64</v>
       </c>
@@ -3088,6 +3078,7 @@
       <c r="E24" s="32"/>
       <c r="F24" s="32"/>
     </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
         <v>56</v>

</xml_diff>